<commit_message>
Added discord server functionality
</commit_message>
<xml_diff>
--- a/timetable.xlsx
+++ b/timetable.xlsx
@@ -1,30 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -43,13 +42,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -374,176 +440,279 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="str">
-        <v>Timings</v>
-      </c>
-      <c r="B1" t="str">
-        <v>09:00 - 10:00</v>
-      </c>
-      <c r="C1" t="str">
-        <v>10:00 - 11:00</v>
-      </c>
-      <c r="D1" t="str">
-        <v>11:00 - 12:00</v>
-      </c>
-      <c r="E1" t="str">
-        <v>12:00 - 13:00</v>
-      </c>
-      <c r="F1" t="str">
-        <v>13:00 - 14:00</v>
-      </c>
-      <c r="G1" t="str">
-        <v>14:00 - 15:00</v>
-      </c>
-      <c r="H1" t="str">
-        <v>15:00 - 17:00</v>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Timings</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>09:00 - 10:00</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>10:00 - 11:00</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>11:00 - 12:00</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>12:00 - 13:00</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>13:00 - 14:00</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>14:00 - 15:00</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>15:00 - 17:00</t>
+        </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="str">
-        <v>Monday</v>
-      </c>
-      <c r="B2" t="str">
-        <v>DC</v>
-      </c>
-      <c r="C2" t="str">
-        <v>CN</v>
-      </c>
-      <c r="D2" t="str">
-        <v>Java</v>
-      </c>
-      <c r="E2" t="str">
-        <v>Lunch</v>
-      </c>
-      <c r="F2" t="str">
-        <v>MWE</v>
-      </c>
-      <c r="G2" t="str">
-        <v>VLSI</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>MPMC</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Java</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Lunch</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>MWE</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>VLSI</t>
+        </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="str">
-        <v>Tuesday</v>
-      </c>
-      <c r="B3" t="str">
-        <v>VLSI</v>
-      </c>
-      <c r="C3" t="str">
-        <v>MPMC</v>
-      </c>
-      <c r="D3" t="str">
-        <v>MWE</v>
-      </c>
-      <c r="E3" t="str">
-        <v>Lunch</v>
-      </c>
-      <c r="F3" t="str">
-        <v>CN</v>
-      </c>
-      <c r="G3" t="str">
-        <v>DC</v>
-      </c>
-      <c r="H3" t="str">
-        <v>R&amp;A</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>VLSI</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>MPMC</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>MWE</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Lunch</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>R&amp;A</t>
+        </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="str">
-        <v>Wednesday</v>
-      </c>
-      <c r="B4" t="str">
-        <v>CN</v>
-      </c>
-      <c r="C4" t="str">
-        <v>Java</v>
-      </c>
-      <c r="D4" t="str">
-        <v>MPMC</v>
-      </c>
-      <c r="E4" t="str">
-        <v>Lunch</v>
-      </c>
-      <c r="F4" t="str">
-        <v>VLSI</v>
-      </c>
-      <c r="G4" t="str">
-        <v>DC</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Java</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>MPMC</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Lunch</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>VLSI</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>DC</t>
+        </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="str">
-        <v>Thursday</v>
-      </c>
-      <c r="B5" t="str">
-        <v>MPMC</v>
-      </c>
-      <c r="C5" t="str">
-        <v>CN</v>
-      </c>
-      <c r="D5" t="str">
-        <v>Java</v>
-      </c>
-      <c r="E5" t="str">
-        <v>Lunch</v>
-      </c>
-      <c r="F5" t="str">
-        <v>PDSS</v>
-      </c>
-      <c r="G5" t="str">
-        <v>PDSS</v>
-      </c>
-      <c r="H5" t="str">
-        <v>R&amp;A</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>MPMC</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Java</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Lunch</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>PDSS</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>PDSS</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>R&amp;A</t>
+        </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="str">
-        <v>Friday</v>
-      </c>
-      <c r="B6" t="str">
-        <v>MWE</v>
-      </c>
-      <c r="C6" t="str">
-        <v>MPMC</v>
-      </c>
-      <c r="D6" t="str">
-        <v>DC</v>
-      </c>
-      <c r="E6" t="str">
-        <v>Lunch</v>
-      </c>
-      <c r="F6" t="str">
-        <v>OOPSLAB</v>
-      </c>
-      <c r="G6" t="str">
-        <v>OOPSLAB</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>MWE</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>MPMC</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>DC</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Lunch</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>OOPSLAB</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>OOPSLAB</t>
+        </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="str">
-        <v>Saturday</v>
-      </c>
-      <c r="B7" t="str">
-        <v>VLSI</v>
-      </c>
-      <c r="C7" t="str">
-        <v>MWE</v>
-      </c>
-      <c r="D7" t="str">
-        <v>Java</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Saturday</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>VLSI</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>MWE</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Java</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H7"/>
-  </ignoredErrors>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed issues with changes made by google
</commit_message>
<xml_diff>
--- a/timetable.xlsx
+++ b/timetable.xlsx
@@ -403,7 +403,7 @@
         <v>14:00 - 15:00</v>
       </c>
       <c r="H1" t="str">
-        <v>15:00 - 17:00</v>
+        <v>15:00 - 23:00</v>
       </c>
     </row>
     <row r="2">
@@ -469,13 +469,16 @@
         <v>MPMC</v>
       </c>
       <c r="E4" t="str">
-        <v>Lunch</v>
+        <v>TEST</v>
       </c>
       <c r="F4" t="str">
-        <v>VLSI</v>
+        <v>TEST</v>
       </c>
       <c r="G4" t="str">
-        <v>DC</v>
+        <v>TEST</v>
+      </c>
+      <c r="H4" t="str">
+        <v>TEST</v>
       </c>
     </row>
     <row r="5">

</xml_diff>